<commit_message>
adding modified file to dev
</commit_message>
<xml_diff>
--- a/Sheet/Shree jyotirling fund Sheet.xlsx
+++ b/Sheet/Shree jyotirling fund Sheet.xlsx
@@ -2499,13 +2499,13 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2513,6 +2513,24 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2531,24 +2549,6 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="14" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="14" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="14" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="14" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -8647,11 +8647,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1179650720"/>
-        <c:axId val="1179651264"/>
+        <c:axId val="916918688"/>
+        <c:axId val="916919232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1179650720"/>
+        <c:axId val="916918688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8693,7 +8693,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1179651264"/>
+        <c:crossAx val="916919232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8701,7 +8701,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1179651264"/>
+        <c:axId val="916919232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8751,7 +8751,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1179650720"/>
+        <c:crossAx val="916918688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9359,7 +9359,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9402,7 +9402,7 @@
         <xdr:cNvPr id="3" name="Picture 2" descr="Fire Ceremony Dattatreya Jayanti Havan | Lilleoru.ee">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9466,7 +9466,7 @@
         <xdr:cNvPr id="2" name="Picture 1" descr="Jotiba Desktop Wallpaper of God \u2013 Free wallpaper download ...">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9535,7 +9535,7 @@
         <xdr:cNvPr id="2" name="Picture 1" descr="Fire Ceremony Dattatreya Jayanti Havan | Lilleoru.ee">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9585,7 +9585,7 @@
         <xdr:cNvPr id="3" name="Picture 2" descr="Jotiba Desktop Wallpaper of God \u2013 Free wallpaper download ...">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12050,7 +12050,7 @@
   <dimension ref="I7:AP64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AC37" zoomScale="78" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="AJ55" sqref="AJ55"/>
+      <selection activeCell="AJ54" sqref="AJ54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -16182,12 +16182,10 @@
       <c r="AI54" s="127">
         <v>200</v>
       </c>
-      <c r="AJ54" s="128">
-        <v>200</v>
-      </c>
+      <c r="AJ54" s="128"/>
       <c r="AK54" s="129">
         <f>SUM(Table35[[#This Row],[JAN]:[VYAJ]])</f>
-        <v>5000</v>
+        <v>4800</v>
       </c>
       <c r="AL54" s="128"/>
       <c r="AM54" s="128"/>
@@ -16799,11 +16797,11 @@
       </c>
       <c r="AJ60" s="133">
         <f>SUBTOTAL(109,Table35[VYAJ])</f>
-        <v>157130</v>
+        <v>156930</v>
       </c>
       <c r="AK60" s="133">
         <f>SUM(Table35[TOTAL(V^2)])</f>
-        <v>1038130</v>
+        <v>1037930</v>
       </c>
       <c r="AL60" s="133">
         <f>SUM(Table35[KARJ])</f>
@@ -16831,7 +16829,7 @@
       <c r="J62" s="147"/>
       <c r="K62" s="74">
         <f>Table35[[#Totals],[TOTAL(V^2)]]-Table35[[#Totals],[TOTAL]]+Table35[[#Totals],[DAND]]</f>
-        <v>605260</v>
+        <v>605060</v>
       </c>
     </row>
     <row r="64" spans="9:42">
@@ -18029,17 +18027,17 @@
     </row>
     <row r="5" spans="2:20" ht="18">
       <c r="B5" s="114"/>
-      <c r="C5" s="162" t="s">
+      <c r="C5" s="151" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="162"/>
-      <c r="E5" s="162"/>
-      <c r="F5" s="162"/>
-      <c r="G5" s="162"/>
-      <c r="H5" s="162"/>
-      <c r="I5" s="162"/>
-      <c r="J5" s="162"/>
-      <c r="K5" s="162"/>
+      <c r="D5" s="151"/>
+      <c r="E5" s="151"/>
+      <c r="F5" s="151"/>
+      <c r="G5" s="151"/>
+      <c r="H5" s="151"/>
+      <c r="I5" s="151"/>
+      <c r="J5" s="151"/>
+      <c r="K5" s="151"/>
       <c r="L5" s="116"/>
       <c r="Q5">
         <f>IF(ISNUMBER(SEARCH($E$11,R5)),MAX($Q$1:Q4)+1,0)</f>
@@ -18055,15 +18053,15 @@
     </row>
     <row r="6" spans="2:20" ht="18">
       <c r="B6" s="114"/>
-      <c r="C6" s="162"/>
-      <c r="D6" s="162"/>
-      <c r="E6" s="162"/>
-      <c r="F6" s="162"/>
-      <c r="G6" s="162"/>
-      <c r="H6" s="162"/>
-      <c r="I6" s="162"/>
-      <c r="J6" s="162"/>
-      <c r="K6" s="162"/>
+      <c r="C6" s="151"/>
+      <c r="D6" s="151"/>
+      <c r="E6" s="151"/>
+      <c r="F6" s="151"/>
+      <c r="G6" s="151"/>
+      <c r="H6" s="151"/>
+      <c r="I6" s="151"/>
+      <c r="J6" s="151"/>
+      <c r="K6" s="151"/>
       <c r="L6" s="116"/>
       <c r="Q6">
         <f>IF(ISNUMBER(SEARCH($E$11,R6)),MAX($Q$1:Q5)+1,0)</f>
@@ -18079,15 +18077,15 @@
     </row>
     <row r="7" spans="2:20" ht="18">
       <c r="B7" s="114"/>
-      <c r="C7" s="162"/>
-      <c r="D7" s="162"/>
-      <c r="E7" s="162"/>
-      <c r="F7" s="162"/>
-      <c r="G7" s="162"/>
-      <c r="H7" s="162"/>
-      <c r="I7" s="162"/>
-      <c r="J7" s="162"/>
-      <c r="K7" s="162"/>
+      <c r="C7" s="151"/>
+      <c r="D7" s="151"/>
+      <c r="E7" s="151"/>
+      <c r="F7" s="151"/>
+      <c r="G7" s="151"/>
+      <c r="H7" s="151"/>
+      <c r="I7" s="151"/>
+      <c r="J7" s="151"/>
+      <c r="K7" s="151"/>
       <c r="L7" s="116"/>
       <c r="Q7">
         <f>IF(ISNUMBER(SEARCH($E$11,R7)),MAX($Q$1:Q6)+1,0)</f>
@@ -18103,17 +18101,17 @@
     </row>
     <row r="8" spans="2:20" ht="14.4" customHeight="1">
       <c r="B8" s="114"/>
-      <c r="C8" s="163" t="s">
+      <c r="C8" s="152" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="163"/>
-      <c r="H8" s="163"/>
-      <c r="I8" s="163"/>
-      <c r="J8" s="163"/>
-      <c r="K8" s="163"/>
+      <c r="D8" s="152"/>
+      <c r="E8" s="152"/>
+      <c r="F8" s="152"/>
+      <c r="G8" s="152"/>
+      <c r="H8" s="152"/>
+      <c r="I8" s="152"/>
+      <c r="J8" s="152"/>
+      <c r="K8" s="152"/>
       <c r="L8" s="116"/>
       <c r="Q8">
         <f>IF(ISNUMBER(SEARCH($E$11,R8)),MAX($Q$1:Q7)+1,0)</f>
@@ -18129,15 +18127,15 @@
     </row>
     <row r="9" spans="2:20" ht="15" customHeight="1">
       <c r="B9" s="114"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="163"/>
-      <c r="H9" s="163"/>
-      <c r="I9" s="163"/>
-      <c r="J9" s="163"/>
-      <c r="K9" s="163"/>
+      <c r="C9" s="152"/>
+      <c r="D9" s="152"/>
+      <c r="E9" s="152"/>
+      <c r="F9" s="152"/>
+      <c r="G9" s="152"/>
+      <c r="H9" s="152"/>
+      <c r="I9" s="152"/>
+      <c r="J9" s="152"/>
+      <c r="K9" s="152"/>
       <c r="L9" s="116"/>
       <c r="Q9">
         <f>IF(ISNUMBER(SEARCH($E$11,R9)),MAX($Q$1:Q8)+1,0)</f>
@@ -18177,17 +18175,17 @@
     </row>
     <row r="11" spans="2:20" ht="28.8" thickBot="1">
       <c r="B11" s="114"/>
-      <c r="C11" s="164" t="s">
+      <c r="C11" s="153" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="164"/>
-      <c r="E11" s="165" t="s">
+      <c r="D11" s="153"/>
+      <c r="E11" s="156" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="166"/>
-      <c r="G11" s="166"/>
-      <c r="H11" s="166"/>
-      <c r="I11" s="167"/>
+      <c r="F11" s="157"/>
+      <c r="G11" s="157"/>
+      <c r="H11" s="157"/>
+      <c r="I11" s="158"/>
       <c r="J11" s="115"/>
       <c r="K11" s="115"/>
       <c r="L11" s="116"/>
@@ -18207,9 +18205,9 @@
       <c r="B12" s="114"/>
       <c r="C12" s="115"/>
       <c r="D12" s="115"/>
-      <c r="E12" s="158"/>
-      <c r="F12" s="158"/>
-      <c r="G12" s="158"/>
+      <c r="E12" s="164"/>
+      <c r="F12" s="164"/>
+      <c r="G12" s="164"/>
       <c r="H12" s="115"/>
       <c r="I12" s="115"/>
       <c r="J12" s="115"/>
@@ -18228,20 +18226,20 @@
       </c>
     </row>
     <row r="13" spans="2:20" ht="25.8" thickBot="1">
-      <c r="B13" s="151" t="s">
+      <c r="B13" s="160" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="152"/>
-      <c r="D13" s="152"/>
-      <c r="E13" s="153"/>
+      <c r="C13" s="159"/>
+      <c r="D13" s="159"/>
+      <c r="E13" s="161"/>
       <c r="F13" s="154">
         <f>_xlfn.IFNA(VLOOKUP(E11,Sheet5!K16:AO59,2,0),0)</f>
         <v>600</v>
       </c>
       <c r="G13" s="155"/>
       <c r="H13" s="115"/>
-      <c r="I13" s="152"/>
-      <c r="J13" s="152"/>
+      <c r="I13" s="159"/>
+      <c r="J13" s="159"/>
       <c r="K13" s="115"/>
       <c r="L13" s="115"/>
       <c r="Q13">
@@ -18281,12 +18279,12 @@
       </c>
     </row>
     <row r="15" spans="2:20" ht="25.8" thickBot="1">
-      <c r="B15" s="151" t="s">
+      <c r="B15" s="160" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="152"/>
-      <c r="D15" s="152"/>
-      <c r="E15" s="153"/>
+      <c r="C15" s="159"/>
+      <c r="D15" s="159"/>
+      <c r="E15" s="161"/>
       <c r="F15" s="154">
         <f>_xlfn.IFNA(VLOOKUP(E11,Sheet5!K16:AO59,27,0),0)</f>
         <v>22680</v>
@@ -18310,9 +18308,9 @@
       </c>
     </row>
     <row r="16" spans="2:20" ht="18.600000000000001" thickBot="1">
-      <c r="B16" s="156"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
+      <c r="B16" s="162"/>
+      <c r="C16" s="163"/>
+      <c r="D16" s="163"/>
       <c r="E16" s="115"/>
       <c r="F16" s="115"/>
       <c r="G16" s="115"/>
@@ -18334,12 +18332,12 @@
       </c>
     </row>
     <row r="17" spans="2:19" ht="25.8" thickBot="1">
-      <c r="B17" s="151" t="s">
+      <c r="B17" s="160" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="152"/>
-      <c r="D17" s="152"/>
-      <c r="E17" s="153"/>
+      <c r="C17" s="159"/>
+      <c r="D17" s="159"/>
+      <c r="E17" s="161"/>
       <c r="F17" s="154">
         <f>_xlfn.IFNA(VLOOKUP(E11,Sheet5!K16:AO59,26,0),0)</f>
         <v>8280</v>
@@ -18387,12 +18385,12 @@
       </c>
     </row>
     <row r="19" spans="2:19" ht="25.8" thickBot="1">
-      <c r="B19" s="151" t="s">
+      <c r="B19" s="160" t="s">
         <v>97</v>
       </c>
-      <c r="C19" s="152"/>
-      <c r="D19" s="152"/>
-      <c r="E19" s="153"/>
+      <c r="C19" s="159"/>
+      <c r="D19" s="159"/>
+      <c r="E19" s="161"/>
       <c r="F19" s="154">
         <f>_xlfn.IFNA(VLOOKUP(E11,Sheet5!K16:AO59,28,0),0)</f>
         <v>61000</v>
@@ -18440,12 +18438,12 @@
       </c>
     </row>
     <row r="21" spans="2:19" ht="25.8" thickBot="1">
-      <c r="B21" s="159" t="s">
+      <c r="B21" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="C21" s="160"/>
-      <c r="D21" s="160"/>
-      <c r="E21" s="161"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="166"/>
+      <c r="E21" s="167"/>
       <c r="F21" s="154">
         <f>_xlfn.IFNA(VLOOKUP(E11,Sheet5!K16:AO59,29,0),0)</f>
         <v>61000</v>
@@ -18493,12 +18491,12 @@
       </c>
     </row>
     <row r="23" spans="2:19" ht="25.8" thickBot="1">
-      <c r="B23" s="151" t="s">
+      <c r="B23" s="160" t="s">
         <v>254</v>
       </c>
-      <c r="C23" s="152"/>
-      <c r="D23" s="152"/>
-      <c r="E23" s="153"/>
+      <c r="C23" s="159"/>
+      <c r="D23" s="159"/>
+      <c r="E23" s="161"/>
       <c r="F23" s="154">
         <f>_xlfn.IFNA(VLOOKUP(E11,Sheet5!K16:AO59,30,0),0)</f>
         <v>0</v>
@@ -18831,13 +18829,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C5:K7"/>
-    <mergeCell ref="C8:K9"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="E11:I11"/>
-    <mergeCell ref="I13:J13"/>
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="B16:D16"/>
@@ -18850,6 +18841,13 @@
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B21:E21"/>
+    <mergeCell ref="C5:K7"/>
+    <mergeCell ref="C8:K9"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="I13:J13"/>
   </mergeCells>
   <conditionalFormatting sqref="R2:R36">
     <cfRule type="expression" dxfId="180" priority="4">

</xml_diff>